<commit_message>
20200403{Start a new day_1}
</commit_message>
<xml_diff>
--- a/2020/4/Tasks.xlsx
+++ b/2020/4/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hall-of-FAME-and-SHAME\2020\4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2D34B4-0D9A-44C0-B5DE-7AB26313BA7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A4CD03-D753-4F75-9A18-D11ABDBE5962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>BPM Lecture 4</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Security L4</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Take More time as video delivery and understood the actual end is 1:52</t>
+  </si>
+  <si>
+    <t>Actual Start</t>
   </si>
 </sst>
 </file>
@@ -122,10 +131,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,9 +426,10 @@
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" customWidth="1"/>
     <col min="6" max="6" width="71.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -438,551 +448,572 @@
       <c r="F1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>43924</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>0.125</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>6.25E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.12638888888888888</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>0.1875</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>0.27083333333333331</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>0.375</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>0.125</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
       <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>2.7777777777777776E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
       <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>0.20833333333333334</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
       <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>0.5</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
         <v>43925</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
+      <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>43926</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
+      <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
+      <c r="A21" s="2"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
+      <c r="A22" s="2"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
+      <c r="A23" s="2"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+      <c r="A24" s="2">
         <v>43927</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
+      <c r="A25" s="2"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
+      <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
+      <c r="A27" s="2"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
+      <c r="A28" s="2"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+      <c r="A29" s="2">
         <v>43928</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
+      <c r="A30" s="2"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
+      <c r="A31" s="2"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
+      <c r="A32" s="2"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
+      <c r="A33" s="2"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
+      <c r="A34" s="2">
         <v>43929</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
+      <c r="A35" s="2"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
+      <c r="A36" s="2"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
+      <c r="A37" s="2"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
+      <c r="A38" s="2"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
+      <c r="A39" s="2">
         <v>43930</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
+      <c r="A40" s="2"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
+      <c r="A41" s="2"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
+      <c r="A42" s="2"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
+      <c r="A43" s="2"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
+      <c r="A44" s="2">
         <v>43931</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
+      <c r="A45" s="2"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
+      <c r="A46" s="2"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
+      <c r="A47" s="2"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
+      <c r="A48" s="2"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
+      <c r="A49" s="2">
         <v>43932</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
+      <c r="A50" s="2"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
+      <c r="A51" s="2"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
+      <c r="A52" s="2"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
+      <c r="A53" s="2"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
+      <c r="A54" s="2">
         <v>43933</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
+      <c r="A55" s="2"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
+      <c r="A56" s="2"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
+      <c r="A57" s="2"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
+      <c r="A58" s="2"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
+      <c r="A59" s="2">
         <v>43934</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
+      <c r="A60" s="2"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="1"/>
+      <c r="A61" s="2"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
+      <c r="A62" s="2"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
+      <c r="A63" s="2"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
+      <c r="A64" s="2">
         <v>43935</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
+      <c r="A65" s="2"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1"/>
+      <c r="A66" s="2"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
+      <c r="A67" s="2"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
+      <c r="A68" s="2"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
+      <c r="A69" s="2">
         <v>43936</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
+      <c r="A70" s="2"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
+      <c r="A71" s="2"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="1"/>
+      <c r="A72" s="2"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1"/>
+      <c r="A73" s="2"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1">
+      <c r="A74" s="2">
         <v>43937</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="1"/>
+      <c r="A75" s="2"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="1"/>
+      <c r="A76" s="2"/>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
+      <c r="A77" s="2"/>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="1"/>
+      <c r="A78" s="2"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="1">
+      <c r="A79" s="2">
         <v>43938</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="1"/>
+      <c r="A80" s="2"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="1"/>
+      <c r="A81" s="2"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="1"/>
+      <c r="A82" s="2"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
+      <c r="A83" s="2"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="1">
+      <c r="A84" s="2">
         <v>43939</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="1"/>
+      <c r="A85" s="2"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="1"/>
+      <c r="A86" s="2"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
+      <c r="A87" s="2"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
+      <c r="A88" s="2"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="1">
+      <c r="A89" s="2">
         <v>43940</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="1"/>
+      <c r="A90" s="2"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="1"/>
+      <c r="A91" s="2"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="1"/>
+      <c r="A92" s="2"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="1"/>
+      <c r="A93" s="2"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="1">
+      <c r="A94" s="2">
         <v>43941</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="1"/>
+      <c r="A95" s="2"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="1"/>
+      <c r="A96" s="2"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="1"/>
+      <c r="A97" s="2"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="1"/>
+      <c r="A98" s="2"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="1">
+      <c r="A99" s="2">
         <v>43942</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="1"/>
+      <c r="A100" s="2"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="1"/>
+      <c r="A101" s="2"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="1"/>
+      <c r="A102" s="2"/>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="1"/>
+      <c r="A103" s="2"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="1">
+      <c r="A104" s="2">
         <v>43943</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" s="1"/>
+      <c r="A105" s="2"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" s="1"/>
+      <c r="A106" s="2"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" s="1"/>
+      <c r="A107" s="2"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="1"/>
+      <c r="A108" s="2"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" s="1">
+      <c r="A109" s="2">
         <v>43944</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" s="1"/>
+      <c r="A110" s="2"/>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" s="1"/>
+      <c r="A111" s="2"/>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" s="1"/>
+      <c r="A112" s="2"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" s="1"/>
+      <c r="A113" s="2"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" s="1">
+      <c r="A114" s="2">
         <v>43945</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" s="1"/>
+      <c r="A115" s="2"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" s="1"/>
+      <c r="A116" s="2"/>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117" s="1"/>
+      <c r="A117" s="2"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" s="1"/>
+      <c r="A118" s="2"/>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119" s="1">
+      <c r="A119" s="2">
         <v>43946</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" s="1"/>
+      <c r="A120" s="2"/>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" s="1"/>
+      <c r="A121" s="2"/>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122" s="1"/>
+      <c r="A122" s="2"/>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123" s="1"/>
+      <c r="A123" s="2"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" s="1">
+      <c r="A124" s="2">
         <v>43947</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" s="1"/>
+      <c r="A125" s="2"/>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" s="1"/>
+      <c r="A126" s="2"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" s="1"/>
+      <c r="A127" s="2"/>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" s="1"/>
+      <c r="A128" s="2"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129" s="1">
+      <c r="A129" s="2">
         <v>43948</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="1"/>
+      <c r="A130" s="2"/>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" s="1"/>
+      <c r="A131" s="2"/>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" s="1"/>
+      <c r="A132" s="2"/>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" s="1"/>
+      <c r="A133" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A34:A38"/>
     <mergeCell ref="A129:A133"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="A99:A103"/>
@@ -999,15 +1030,6 @@
     <mergeCell ref="A94:A98"/>
     <mergeCell ref="A39:A43"/>
     <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A59:A63"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="A34:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
20200403{Start a new day_2}
</commit_message>
<xml_diff>
--- a/2020/4/Tasks.xlsx
+++ b/2020/4/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hall-of-FAME-and-SHAME\2020\4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A4CD03-D753-4F75-9A18-D11ABDBE5962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3396D42-A23E-4D3A-BD0D-4291719059C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>BPM Lecture 4</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Actual Start</t>
+  </si>
+  <si>
+    <t>Alhamdu Li Allah</t>
+  </si>
+  <si>
+    <t>Quantitative anlysis of process {flow Analysis of time}</t>
   </si>
 </sst>
 </file>
@@ -418,7 +424,7 @@
   <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,6 +492,15 @@
       <c r="D3" s="1">
         <v>6.25E-2</v>
       </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.20833333333333334</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
@@ -495,6 +510,15 @@
       <c r="D4" s="1">
         <v>1.3888888888888888E-2</v>
       </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.20138888888888887</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -1005,15 +1029,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A59:A63"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="A34:A38"/>
     <mergeCell ref="A129:A133"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="A99:A103"/>
@@ -1030,6 +1045,15 @@
     <mergeCell ref="A94:A98"/>
     <mergeCell ref="A39:A43"/>
     <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A34:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
20200403{Start a new day_3}
</commit_message>
<xml_diff>
--- a/2020/4/Tasks.xlsx
+++ b/2020/4/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hall-of-FAME-and-SHAME\2020\4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3396D42-A23E-4D3A-BD0D-4291719059C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B44F8EB-93CC-4525-B523-002337C3F546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>BPM Lecture 4</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Lunch</t>
   </si>
   <si>
-    <t>Programming Blazor</t>
-  </si>
-  <si>
     <t>Praying Maghrab</t>
   </si>
   <si>
@@ -100,6 +97,21 @@
   </si>
   <si>
     <t>Quantitative anlysis of process {flow Analysis of time}</t>
+  </si>
+  <si>
+    <t>Half of it in the product cipher encryption</t>
+  </si>
+  <si>
+    <t>A headache on my head and I can't forgive myself</t>
+  </si>
+  <si>
+    <t>Alhamdu Li Allah =&gt; sleeping period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alhamdu Li Allah </t>
+  </si>
+  <si>
+    <t>Programming GP</t>
   </si>
 </sst>
 </file>
@@ -424,7 +436,7 @@
   <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,7 +467,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -472,10 +484,10 @@
         <v>6.25E-2</v>
       </c>
       <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
         <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
       </c>
       <c r="G2" s="1">
         <v>0.12638888888888888</v>
@@ -493,10 +505,10 @@
         <v>6.25E-2</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1">
         <v>0.20833333333333334</v>
@@ -511,10 +523,10 @@
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1">
         <v>0.20138888888888887</v>
@@ -531,6 +543,15 @@
       <c r="D5" s="1">
         <v>6.25E-2</v>
       </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.34722222222222227</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -543,6 +564,15 @@
       <c r="D6" s="1">
         <v>0.29166666666666669</v>
       </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.41666666666666669</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
@@ -555,6 +585,15 @@
       <c r="D7" s="1">
         <v>1.3888888888888888E-2</v>
       </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.16666666666666666</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
@@ -564,6 +603,15 @@
       <c r="D8" s="1">
         <v>1.3888888888888888E-2</v>
       </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.17361111111111113</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
@@ -580,7 +628,7 @@
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1">
         <v>0.20833333333333334</v>
@@ -592,7 +640,7 @@
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1">
         <v>1.3888888888888888E-2</v>
@@ -601,7 +649,7 @@
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1">
         <v>1.3888888888888888E-2</v>
@@ -610,7 +658,7 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1">
         <v>0.5</v>
@@ -1029,6 +1077,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A34:A38"/>
     <mergeCell ref="A129:A133"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="A99:A103"/>
@@ -1045,15 +1102,6 @@
     <mergeCell ref="A94:A98"/>
     <mergeCell ref="A39:A43"/>
     <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A59:A63"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="A34:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
20200404{Adding The 4th april_1}
</commit_message>
<xml_diff>
--- a/2020/4/Tasks.xlsx
+++ b/2020/4/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hall-of-FAME-and-SHAME\2020\4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600AE386-DBAF-4C42-9DDF-D0FC6F1AA792}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184371B1-CE1E-4A12-AEF2-50E61376DA20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>BPM Lecture 4</t>
   </si>
@@ -132,7 +132,10 @@
     <t>Data Mining Lec3</t>
   </si>
   <si>
-    <t>Data Mining Algorithms Aggregation</t>
+    <t>PluralSight Data Scraping</t>
+  </si>
+  <si>
+    <t>2/3 of it in the lecture to the Symmetric vs Skewed data</t>
   </si>
 </sst>
 </file>
@@ -177,11 +180,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +468,7 @@
   <dimension ref="A1:G140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,7 +504,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>43924</v>
       </c>
       <c r="B2" t="s">
@@ -524,7 +527,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -545,7 +548,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -563,7 +566,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+      <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -584,7 +587,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -605,7 +608,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -626,7 +629,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -644,7 +647,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -661,26 +664,26 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3" t="s">
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0.25</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+      <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -695,7 +698,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -709,26 +712,26 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
+    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>0.5</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>6.25E-2</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="4">
         <v>43925</v>
       </c>
       <c r="B14" t="s">
@@ -748,7 +751,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>29</v>
       </c>
@@ -766,7 +769,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
+      <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>30</v>
       </c>
@@ -776,33 +779,39 @@
       <c r="D16" s="1">
         <v>6.25E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.50486111111111109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="1">
-        <v>6.25E-2</v>
+        <v>9.0277777777777776E-2</v>
       </c>
       <c r="D17" s="1">
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="1">
-        <v>0.16666666666666666</v>
+        <v>0.1875</v>
       </c>
       <c r="D18" s="1">
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
       <c r="B19" t="s">
         <v>33</v>
       </c>
@@ -810,11 +819,11 @@
         <v>0.25</v>
       </c>
       <c r="D19" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -822,9 +831,18 @@
       <c r="D20" s="1">
         <v>1.3888888888888888E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.51388888888888895</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>12</v>
       </c>
@@ -833,8 +851,8 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
       <c r="B22" t="s">
         <v>14</v>
       </c>
@@ -843,8 +861,8 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
       <c r="B23" t="s">
         <v>15</v>
       </c>
@@ -852,8 +870,8 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
       <c r="B24" t="s">
         <v>13</v>
       </c>
@@ -861,8 +879,8 @@
         <v>2.7777777777777776E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
       <c r="B25" t="s">
         <v>26</v>
       </c>
@@ -873,396 +891,396 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
         <v>43926</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
         <v>43927</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
+      <c r="A33" s="4"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
+      <c r="A34" s="4"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
+      <c r="A35" s="4"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
+      <c r="A36" s="4">
         <v>43928</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
+      <c r="A37" s="4"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
+      <c r="A38" s="4"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
+      <c r="A39" s="4"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
+      <c r="A40" s="4"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
+      <c r="A41" s="4">
         <v>43929</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2"/>
+      <c r="A42" s="4"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
+      <c r="A43" s="4"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
+      <c r="A44" s="4"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2"/>
+      <c r="A45" s="4"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
+      <c r="A46" s="4">
         <v>43930</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
+      <c r="A47" s="4"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2"/>
+      <c r="A48" s="4"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
+      <c r="A49" s="4"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2"/>
+      <c r="A50" s="4"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
+      <c r="A51" s="4">
         <v>43931</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2"/>
+      <c r="A52" s="4"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2"/>
+      <c r="A53" s="4"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2"/>
+      <c r="A54" s="4"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="2"/>
+      <c r="A55" s="4"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
+      <c r="A56" s="4">
         <v>43932</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="2"/>
+      <c r="A57" s="4"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="2"/>
+      <c r="A58" s="4"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2"/>
+      <c r="A59" s="4"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="2"/>
+      <c r="A60" s="4"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
+      <c r="A61" s="4">
         <v>43933</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="2"/>
+      <c r="A62" s="4"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="2"/>
+      <c r="A63" s="4"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="2"/>
+      <c r="A64" s="4"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="2"/>
+      <c r="A65" s="4"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="2">
+      <c r="A66" s="4">
         <v>43934</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="2"/>
+      <c r="A67" s="4"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="2"/>
+      <c r="A68" s="4"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="2"/>
+      <c r="A69" s="4"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="2"/>
+      <c r="A70" s="4"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
+      <c r="A71" s="4">
         <v>43935</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="2"/>
+      <c r="A72" s="4"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="2"/>
+      <c r="A73" s="4"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="2"/>
+      <c r="A74" s="4"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="2"/>
+      <c r="A75" s="4"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="2">
+      <c r="A76" s="4">
         <v>43936</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="2"/>
+      <c r="A77" s="4"/>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="2"/>
+      <c r="A78" s="4"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="2"/>
+      <c r="A79" s="4"/>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="2"/>
+      <c r="A80" s="4"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="2">
+      <c r="A81" s="4">
         <v>43937</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="2"/>
+      <c r="A82" s="4"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="2"/>
+      <c r="A83" s="4"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="2"/>
+      <c r="A84" s="4"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="2"/>
+      <c r="A85" s="4"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2">
+      <c r="A86" s="4">
         <v>43938</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="2"/>
+      <c r="A87" s="4"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="2"/>
+      <c r="A88" s="4"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="2"/>
+      <c r="A89" s="4"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="2"/>
+      <c r="A90" s="4"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="2">
+      <c r="A91" s="4">
         <v>43939</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="2"/>
+      <c r="A92" s="4"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="2"/>
+      <c r="A93" s="4"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="2"/>
+      <c r="A94" s="4"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="2"/>
+      <c r="A95" s="4"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="2">
+      <c r="A96" s="4">
         <v>43940</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="2"/>
+      <c r="A97" s="4"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="2"/>
+      <c r="A98" s="4"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="2"/>
+      <c r="A99" s="4"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="2"/>
+      <c r="A100" s="4"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="2">
+      <c r="A101" s="4">
         <v>43941</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="2"/>
+      <c r="A102" s="4"/>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="2"/>
+      <c r="A103" s="4"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="2"/>
+      <c r="A104" s="4"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" s="2"/>
+      <c r="A105" s="4"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" s="2">
+      <c r="A106" s="4">
         <v>43942</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" s="2"/>
+      <c r="A107" s="4"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="2"/>
+      <c r="A108" s="4"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" s="2"/>
+      <c r="A109" s="4"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" s="2"/>
+      <c r="A110" s="4"/>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" s="2">
+      <c r="A111" s="4">
         <v>43943</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" s="2"/>
+      <c r="A112" s="4"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" s="2"/>
+      <c r="A113" s="4"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" s="2"/>
+      <c r="A114" s="4"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" s="2"/>
+      <c r="A115" s="4"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" s="2">
+      <c r="A116" s="4">
         <v>43944</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117" s="2"/>
+      <c r="A117" s="4"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" s="2"/>
+      <c r="A118" s="4"/>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119" s="2"/>
+      <c r="A119" s="4"/>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" s="2"/>
+      <c r="A120" s="4"/>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" s="2">
+      <c r="A121" s="4">
         <v>43945</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122" s="2"/>
+      <c r="A122" s="4"/>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123" s="2"/>
+      <c r="A123" s="4"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" s="2"/>
+      <c r="A124" s="4"/>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" s="2"/>
+      <c r="A125" s="4"/>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" s="2">
+      <c r="A126" s="4">
         <v>43946</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" s="2"/>
+      <c r="A127" s="4"/>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" s="2"/>
+      <c r="A128" s="4"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129" s="2"/>
+      <c r="A129" s="4"/>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="2"/>
+      <c r="A130" s="4"/>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" s="2">
+      <c r="A131" s="4">
         <v>43947</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" s="2"/>
+      <c r="A132" s="4"/>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" s="2"/>
+      <c r="A133" s="4"/>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134" s="2"/>
+      <c r="A134" s="4"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135" s="2"/>
+      <c r="A135" s="4"/>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136" s="2">
+      <c r="A136" s="4">
         <v>43948</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137" s="2"/>
+      <c r="A137" s="4"/>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138" s="2"/>
+      <c r="A138" s="4"/>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139" s="2"/>
+      <c r="A139" s="4"/>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140" s="2"/>
+      <c r="A140" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="25">

</xml_diff>